<commit_message>
Fixed bags. Added OBXList. Add new components. Add metods saved to DB. Refactoring.
</commit_message>
<xml_diff>
--- a/DOC/HL7_and_DBTables.xlsx
+++ b/DOC/HL7_and_DBTables.xlsx
@@ -2,29 +2,33 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DelphiProjects\_Kuhtin\HL7\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="8580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="328">
   <si>
     <t>MSH</t>
   </si>
@@ -842,15 +846,9 @@
     <t>full_name VARCHAR (120)</t>
   </si>
   <si>
-    <t>2.3.2</t>
-  </si>
-  <si>
     <t>DateBirth</t>
   </si>
   <si>
-    <t>2.11.1 + 2.11.2</t>
-  </si>
-  <si>
     <t>1.20</t>
   </si>
   <si>
@@ -972,13 +970,55 @@
   </si>
   <si>
     <t>accession_id INTEGER,</t>
+  </si>
+  <si>
+    <t>date_obtained DATETIME,</t>
+  </si>
+  <si>
+    <t>New Entity on Accession table</t>
+  </si>
+  <si>
+    <t>SpecimenSource  - component 2</t>
+  </si>
+  <si>
+    <t>SpecimenSource  - component 3</t>
+  </si>
+  <si>
+    <t>3.14.2</t>
+  </si>
+  <si>
+    <t>3.14.3</t>
+  </si>
+  <si>
+    <t>I didn’t send you priority table but it is a lookup table for the priority</t>
+  </si>
+  <si>
+    <t>but patient_id from patient table where patient_id = PatientIDInt</t>
+  </si>
+  <si>
+    <t>PatientIDInt (foreign key)</t>
+  </si>
+  <si>
+    <t>http://www.mexi.be/documents/hl7/ch700011.htm#E12E290</t>
+  </si>
+  <si>
+    <t>OBX with TX value type and GDT suffix</t>
+  </si>
+  <si>
+    <t>OBX with TX value type and IMP suffix</t>
+  </si>
+  <si>
+    <t>OBX with TX value type and MDT suffix</t>
+  </si>
+  <si>
+    <t>OBX with TX value type and TCM suffix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -996,8 +1036,34 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1016,6 +1082,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1026,10 +1098,59 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1056,9 +1177,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="49"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="50">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="49" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="48" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1116,7 +1291,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1151,7 +1326,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1336,21 +1511,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F342"/>
+  <dimension ref="A1:H342"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42" customWidth="1"/>
+    <col min="8" max="8" width="65.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>241</v>
       </c>
@@ -1363,11 +1541,11 @@
       <c r="E1" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="14" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1380,9 +1558,9 @@
       <c r="E2" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1395,11 +1573,11 @@
       <c r="E3" t="s">
         <v>245</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1412,11 +1590,11 @@
       <c r="E4" t="s">
         <v>246</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1429,9 +1607,14 @@
       <c r="E5" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1444,11 +1627,11 @@
       <c r="E6" t="s">
         <v>248</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1461,11 +1644,11 @@
       <c r="E7" t="s">
         <v>249</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1478,9 +1661,8 @@
       <c r="E8" t="s">
         <v>250</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1493,11 +1675,11 @@
       <c r="E9" t="s">
         <v>251</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1510,11 +1692,11 @@
       <c r="E10" t="s">
         <v>252</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -1527,9 +1709,8 @@
       <c r="E11" t="s">
         <v>253</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1542,9 +1723,8 @@
       <c r="E12" t="s">
         <v>254</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -1557,11 +1737,11 @@
       <c r="E13" t="s">
         <v>255</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1574,11 +1754,11 @@
       <c r="E14" t="s">
         <v>256</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="18" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1591,11 +1771,11 @@
       <c r="E15" t="s">
         <v>257</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1608,11 +1788,11 @@
       <c r="E16" t="s">
         <v>258</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1625,11 +1805,11 @@
       <c r="E17" t="s">
         <v>259</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1642,9 +1822,8 @@
       <c r="E18" t="s">
         <v>260</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1657,11 +1836,11 @@
       <c r="E19" t="s">
         <v>261</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1674,9 +1853,8 @@
       <c r="E20" t="s">
         <v>262</v>
       </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
@@ -1689,9 +1867,8 @@
       <c r="E21" t="s">
         <v>263</v>
       </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>39</v>
       </c>
@@ -1699,14 +1876,13 @@
         <v>40</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E22" t="s">
         <v>264</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>46</v>
       </c>
@@ -1714,14 +1890,13 @@
         <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E23" t="s">
         <v>265</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
@@ -1729,14 +1904,13 @@
         <v>42</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E24" t="s">
         <v>266</v>
       </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -1744,14 +1918,13 @@
         <v>43</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E25" t="s">
         <v>267</v>
       </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
@@ -1759,14 +1932,13 @@
         <v>44</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E26" t="s">
         <v>268</v>
       </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
@@ -1774,14 +1946,13 @@
         <v>45</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E27" t="s">
         <v>269</v>
       </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>76</v>
       </c>
@@ -1789,14 +1960,13 @@
         <v>77</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E28" t="s">
         <v>270</v>
       </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>81</v>
       </c>
@@ -1804,16 +1974,16 @@
         <v>78</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E29" t="s">
         <v>271</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>82</v>
       </c>
@@ -1824,11 +1994,11 @@
         <v>39</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
@@ -1839,11 +2009,10 @@
         <v>46</v>
       </c>
       <c r="E31" t="s">
-        <v>283</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>51</v>
       </c>
@@ -1854,26 +2023,30 @@
         <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>284</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E33" t="s">
-        <v>285</v>
-      </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>53</v>
       </c>
@@ -1884,11 +2057,10 @@
         <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>286</v>
-      </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>54</v>
       </c>
@@ -1899,11 +2071,16 @@
         <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>287</v>
-      </c>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G35" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>55</v>
       </c>
@@ -1914,11 +2091,10 @@
         <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>288</v>
-      </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>56</v>
       </c>
@@ -1929,11 +2105,16 @@
         <v>52</v>
       </c>
       <c r="E37" t="s">
-        <v>289</v>
-      </c>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+      <c r="G37" t="s">
+        <v>326</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>89</v>
       </c>
@@ -1944,11 +2125,16 @@
         <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>290</v>
-      </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="G38" t="s">
+        <v>325</v>
+      </c>
+      <c r="H38" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>96</v>
       </c>
@@ -1959,11 +2145,10 @@
         <v>54</v>
       </c>
       <c r="E39" t="s">
-        <v>291</v>
-      </c>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>97</v>
       </c>
@@ -1974,11 +2159,10 @@
         <v>55</v>
       </c>
       <c r="E40" t="s">
-        <v>292</v>
-      </c>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>98</v>
       </c>
@@ -1989,11 +2173,10 @@
         <v>56</v>
       </c>
       <c r="E41" t="s">
-        <v>293</v>
-      </c>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>99</v>
       </c>
@@ -2004,11 +2187,10 @@
         <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>294</v>
-      </c>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>100</v>
       </c>
@@ -2021,9 +2203,14 @@
       <c r="E43" t="s">
         <v>264</v>
       </c>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="H43" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -2034,11 +2221,10 @@
         <v>59</v>
       </c>
       <c r="E44" t="s">
-        <v>295</v>
-      </c>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>58</v>
       </c>
@@ -2049,11 +2235,10 @@
         <v>60</v>
       </c>
       <c r="E45" t="s">
-        <v>296</v>
-      </c>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>59</v>
       </c>
@@ -2064,11 +2249,10 @@
         <v>61</v>
       </c>
       <c r="E46" t="s">
-        <v>297</v>
-      </c>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>60</v>
       </c>
@@ -2079,11 +2263,19 @@
         <v>62</v>
       </c>
       <c r="E47" t="s">
-        <v>298</v>
-      </c>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H47" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>61</v>
       </c>
@@ -2094,11 +2286,10 @@
         <v>63</v>
       </c>
       <c r="E48" t="s">
-        <v>299</v>
-      </c>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>62</v>
       </c>
@@ -2109,11 +2300,10 @@
         <v>64</v>
       </c>
       <c r="E49" t="s">
-        <v>300</v>
-      </c>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>63</v>
       </c>
@@ -2124,11 +2314,10 @@
         <v>65</v>
       </c>
       <c r="E50" t="s">
-        <v>301</v>
-      </c>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>64</v>
       </c>
@@ -2139,11 +2328,16 @@
         <v>66</v>
       </c>
       <c r="E51" t="s">
-        <v>302</v>
-      </c>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>65</v>
       </c>
@@ -2154,11 +2348,10 @@
         <v>67</v>
       </c>
       <c r="E52" t="s">
-        <v>303</v>
-      </c>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>66</v>
       </c>
@@ -2169,11 +2362,16 @@
         <v>68</v>
       </c>
       <c r="E53" t="s">
-        <v>304</v>
-      </c>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G53" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>67</v>
       </c>
@@ -2184,11 +2382,10 @@
         <v>69</v>
       </c>
       <c r="E54" t="s">
-        <v>305</v>
-      </c>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>68</v>
       </c>
@@ -2199,11 +2396,11 @@
         <v>120</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F55" s="13"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>69</v>
       </c>
@@ -2214,11 +2411,16 @@
         <v>122</v>
       </c>
       <c r="E56" t="s">
-        <v>308</v>
-      </c>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+      <c r="F56" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>70</v>
       </c>
@@ -2229,11 +2431,16 @@
         <v>165</v>
       </c>
       <c r="E57" t="s">
-        <v>309</v>
-      </c>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+      <c r="F57" s="1">
+        <v>3.12</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>71</v>
       </c>
@@ -2244,11 +2451,16 @@
         <v>166</v>
       </c>
       <c r="E58" t="s">
-        <v>310</v>
-      </c>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+      <c r="F58" s="1">
+        <v>3.36</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>72</v>
       </c>
@@ -2259,11 +2471,19 @@
         <v>167</v>
       </c>
       <c r="E59" t="s">
-        <v>311</v>
-      </c>
-      <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G59" t="s">
+        <v>322</v>
+      </c>
+      <c r="H59" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>73</v>
       </c>
@@ -2274,11 +2494,11 @@
         <v>168</v>
       </c>
       <c r="E60" t="s">
-        <v>312</v>
-      </c>
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>74</v>
       </c>
@@ -2289,11 +2509,10 @@
         <v>169</v>
       </c>
       <c r="E61" t="s">
-        <v>313</v>
-      </c>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>75</v>
       </c>
@@ -2306,9 +2525,8 @@
       <c r="E62" t="s">
         <v>269</v>
       </c>
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>120</v>
       </c>
@@ -2321,9 +2539,8 @@
       <c r="E63" t="s">
         <v>268</v>
       </c>
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>122</v>
       </c>
@@ -2334,11 +2551,10 @@
         <v>172</v>
       </c>
       <c r="E64" t="s">
-        <v>314</v>
-      </c>
-      <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>165</v>
       </c>
@@ -2349,11 +2565,10 @@
         <v>173</v>
       </c>
       <c r="E65" t="s">
-        <v>286</v>
-      </c>
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>166</v>
       </c>
@@ -2364,21 +2579,33 @@
         <v>174</v>
       </c>
       <c r="E66" t="s">
-        <v>315</v>
-      </c>
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D67" s="3"/>
-      <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D67" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E67" t="s">
+        <v>314</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H67" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>168</v>
       </c>
@@ -2386,9 +2613,8 @@
         <v>127</v>
       </c>
       <c r="D68" s="3"/>
-      <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>169</v>
       </c>
@@ -2396,9 +2622,8 @@
         <v>128</v>
       </c>
       <c r="D69" s="3"/>
-      <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>170</v>
       </c>
@@ -2406,9 +2631,8 @@
         <v>129</v>
       </c>
       <c r="D70" s="3"/>
-      <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>171</v>
       </c>
@@ -2416,9 +2640,8 @@
         <v>130</v>
       </c>
       <c r="D71" s="3"/>
-      <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>172</v>
       </c>
@@ -2426,9 +2649,8 @@
         <v>131</v>
       </c>
       <c r="D72" s="3"/>
-      <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>173</v>
       </c>
@@ -2436,9 +2658,8 @@
         <v>132</v>
       </c>
       <c r="D73" s="3"/>
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>174</v>
       </c>
@@ -2446,9 +2667,8 @@
         <v>133</v>
       </c>
       <c r="D74" s="3"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>175</v>
       </c>
@@ -2456,9 +2676,8 @@
         <v>134</v>
       </c>
       <c r="D75" s="3"/>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>176</v>
       </c>
@@ -2466,9 +2685,8 @@
         <v>135</v>
       </c>
       <c r="D76" s="3"/>
-      <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>177</v>
       </c>
@@ -2476,9 +2694,8 @@
         <v>136</v>
       </c>
       <c r="D77" s="3"/>
-      <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>178</v>
       </c>
@@ -2486,9 +2703,8 @@
         <v>137</v>
       </c>
       <c r="D78" s="3"/>
-      <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>179</v>
       </c>
@@ -2496,9 +2712,8 @@
         <v>138</v>
       </c>
       <c r="D79" s="3"/>
-      <c r="F79" s="1"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>180</v>
       </c>
@@ -2506,9 +2721,8 @@
         <v>139</v>
       </c>
       <c r="D80" s="3"/>
-      <c r="F80" s="1"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>181</v>
       </c>
@@ -2516,9 +2730,8 @@
         <v>140</v>
       </c>
       <c r="D81" s="3"/>
-      <c r="F81" s="1"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>182</v>
       </c>
@@ -2526,9 +2739,8 @@
         <v>141</v>
       </c>
       <c r="D82" s="3"/>
-      <c r="F82" s="1"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>183</v>
       </c>
@@ -2536,9 +2748,8 @@
         <v>142</v>
       </c>
       <c r="D83" s="3"/>
-      <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>184</v>
       </c>
@@ -2546,9 +2757,8 @@
         <v>143</v>
       </c>
       <c r="D84" s="3"/>
-      <c r="F84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>185</v>
       </c>
@@ -2556,9 +2766,8 @@
         <v>144</v>
       </c>
       <c r="D85" s="3"/>
-      <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>186</v>
       </c>
@@ -2566,9 +2775,8 @@
         <v>145</v>
       </c>
       <c r="D86" s="3"/>
-      <c r="F86" s="1"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>187</v>
       </c>
@@ -2576,9 +2784,8 @@
         <v>146</v>
       </c>
       <c r="D87" s="3"/>
-      <c r="F87" s="1"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>188</v>
       </c>
@@ -2586,9 +2793,8 @@
         <v>147</v>
       </c>
       <c r="D88" s="3"/>
-      <c r="F88" s="1"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>189</v>
       </c>
@@ -2596,9 +2802,8 @@
         <v>148</v>
       </c>
       <c r="D89" s="3"/>
-      <c r="F89" s="1"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>190</v>
       </c>
@@ -2606,9 +2811,8 @@
         <v>149</v>
       </c>
       <c r="D90" s="3"/>
-      <c r="F90" s="1"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>191</v>
       </c>
@@ -2616,9 +2820,8 @@
         <v>150</v>
       </c>
       <c r="D91" s="3"/>
-      <c r="F91" s="1"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>192</v>
       </c>
@@ -2626,9 +2829,8 @@
         <v>151</v>
       </c>
       <c r="D92" s="3"/>
-      <c r="F92" s="1"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>193</v>
       </c>
@@ -2636,9 +2838,8 @@
         <v>152</v>
       </c>
       <c r="D93" s="3"/>
-      <c r="F93" s="1"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>194</v>
       </c>
@@ -2646,9 +2847,8 @@
         <v>153</v>
       </c>
       <c r="D94" s="3"/>
-      <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>195</v>
       </c>
@@ -2656,9 +2856,8 @@
         <v>154</v>
       </c>
       <c r="D95" s="3"/>
-      <c r="F95" s="1"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>196</v>
       </c>
@@ -2666,9 +2865,8 @@
         <v>155</v>
       </c>
       <c r="D96" s="3"/>
-      <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>197</v>
       </c>
@@ -2676,9 +2874,8 @@
         <v>156</v>
       </c>
       <c r="D97" s="3"/>
-      <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>198</v>
       </c>
@@ -2686,9 +2883,8 @@
         <v>157</v>
       </c>
       <c r="D98" s="3"/>
-      <c r="F98" s="1"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>199</v>
       </c>
@@ -2696,9 +2892,8 @@
         <v>158</v>
       </c>
       <c r="D99" s="3"/>
-      <c r="F99" s="1"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>200</v>
       </c>
@@ -2706,9 +2901,8 @@
         <v>159</v>
       </c>
       <c r="D100" s="3"/>
-      <c r="F100" s="1"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>201</v>
       </c>
@@ -2716,9 +2910,8 @@
         <v>160</v>
       </c>
       <c r="D101" s="3"/>
-      <c r="F101" s="1"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>202</v>
       </c>
@@ -2726,9 +2919,8 @@
         <v>161</v>
       </c>
       <c r="D102" s="3"/>
-      <c r="F102" s="1"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>203</v>
       </c>
@@ -2736,9 +2928,8 @@
         <v>162</v>
       </c>
       <c r="D103" s="3"/>
-      <c r="F103" s="1"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>204</v>
       </c>
@@ -2746,9 +2937,8 @@
         <v>163</v>
       </c>
       <c r="D104" s="3"/>
-      <c r="F104" s="1"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>205</v>
       </c>
@@ -2756,9 +2946,8 @@
         <v>164</v>
       </c>
       <c r="D105" s="3"/>
-      <c r="F105" s="1"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>206</v>
       </c>
@@ -2766,9 +2955,8 @@
         <v>207</v>
       </c>
       <c r="D106" s="3"/>
-      <c r="F106" s="1"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>208</v>
       </c>
@@ -2776,9 +2964,8 @@
         <v>209</v>
       </c>
       <c r="D107" s="3"/>
-      <c r="F107" s="1"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>225</v>
       </c>
@@ -2786,9 +2973,8 @@
         <v>210</v>
       </c>
       <c r="D108" s="3"/>
-      <c r="F108" s="1"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>226</v>
       </c>
@@ -2796,9 +2982,8 @@
         <v>211</v>
       </c>
       <c r="D109" s="3"/>
-      <c r="F109" s="1"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>227</v>
       </c>
@@ -2806,9 +2991,8 @@
         <v>212</v>
       </c>
       <c r="D110" s="3"/>
-      <c r="F110" s="1"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>228</v>
       </c>
@@ -2816,9 +3000,8 @@
         <v>213</v>
       </c>
       <c r="D111" s="3"/>
-      <c r="F111" s="1"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>229</v>
       </c>
@@ -2826,9 +3009,8 @@
         <v>214</v>
       </c>
       <c r="D112" s="3"/>
-      <c r="F112" s="1"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>230</v>
       </c>
@@ -2836,9 +3018,8 @@
         <v>215</v>
       </c>
       <c r="D113" s="3"/>
-      <c r="F113" s="1"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>231</v>
       </c>
@@ -2846,9 +3027,8 @@
         <v>216</v>
       </c>
       <c r="D114" s="3"/>
-      <c r="F114" s="1"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>232</v>
       </c>
@@ -2856,9 +3036,8 @@
         <v>217</v>
       </c>
       <c r="D115" s="3"/>
-      <c r="F115" s="1"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>233</v>
       </c>
@@ -2866,9 +3045,8 @@
         <v>218</v>
       </c>
       <c r="D116" s="3"/>
-      <c r="F116" s="1"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>234</v>
       </c>
@@ -2876,9 +3054,8 @@
         <v>219</v>
       </c>
       <c r="D117" s="3"/>
-      <c r="F117" s="1"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>235</v>
       </c>
@@ -2886,9 +3063,8 @@
         <v>220</v>
       </c>
       <c r="D118" s="3"/>
-      <c r="F118" s="1"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>236</v>
       </c>
@@ -2896,9 +3072,8 @@
         <v>221</v>
       </c>
       <c r="D119" s="3"/>
-      <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>237</v>
       </c>
@@ -2906,9 +3081,8 @@
         <v>222</v>
       </c>
       <c r="D120" s="3"/>
-      <c r="F120" s="1"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>238</v>
       </c>
@@ -2916,9 +3090,8 @@
         <v>223</v>
       </c>
       <c r="D121" s="3"/>
-      <c r="F121" s="1"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>239</v>
       </c>
@@ -2926,128 +3099,113 @@
         <v>224</v>
       </c>
       <c r="D122" s="3"/>
-      <c r="F122" s="1"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="1"/>
       <c r="D123" s="3"/>
-      <c r="F123" s="1"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="1"/>
       <c r="D124" s="3"/>
-      <c r="F124" s="1"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="1"/>
       <c r="D125" s="3"/>
-      <c r="F125" s="1"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="1"/>
       <c r="D126" s="3"/>
-      <c r="F126" s="1"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="1"/>
       <c r="D127" s="3"/>
-      <c r="F127" s="1"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="1"/>
       <c r="D128" s="3"/>
-      <c r="F128" s="1"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="1"/>
       <c r="D129" s="3"/>
-      <c r="F129" s="1"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="1"/>
       <c r="D130" s="3"/>
-      <c r="F130" s="1"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="1"/>
       <c r="D131" s="3"/>
-      <c r="F131" s="1"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="1"/>
       <c r="D132" s="3"/>
-      <c r="F132" s="1"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="1"/>
       <c r="D133" s="3"/>
-      <c r="F133" s="1"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="1"/>
       <c r="D134" s="3"/>
-      <c r="F134" s="1"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="1"/>
       <c r="D135" s="3"/>
-      <c r="F135" s="1"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="1"/>
       <c r="D136" s="3"/>
-      <c r="F136" s="1"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="1"/>
       <c r="D137" s="3"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="1"/>
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="1"/>
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="1"/>
       <c r="D140" s="3"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="1"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="1"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="1"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="1"/>
       <c r="D144" s="2"/>
@@ -3926,7 +4084,37 @@
       <c r="B342" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H37" r:id="rId1" location="E12E290"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>